<commit_message>
intento de union de flujo
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/FlujosMCSS.xlsx
+++ b/web-automation-framework/src/main/resources/excel/FlujosMCSS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr documentId="13_ncr:1_{37D8D553-F8C8-49C2-9BE9-63B5D613167A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView windowHeight="2760" windowWidth="14670" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Login" r:id="rId1" sheetId="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>TC1</t>
   </si>
@@ -167,17 +168,17 @@
     <t>Florida</t>
   </si>
   <si>
-    <t>ricardofort26543374@gmail.com</t>
+    <t>ric4rdof0rt23224@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +220,10 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,7 +246,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -260,7 +265,8 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
@@ -541,11 +547,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +737,7 @@
     <row customFormat="1" r="71" s="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId1" ref="C2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
@@ -739,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -869,7 +875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>